<commit_message>
Separated movement from generation, modified click routine
</commit_message>
<xml_diff>
--- a/Adventurers-Inc/Assets/Data/Names/Names.xlsx
+++ b/Adventurers-Inc/Assets/Data/Names/Names.xlsx
@@ -107,9 +107,6 @@
     <t>Maverick</t>
   </si>
   <si>
-    <t>Eiikichi</t>
-  </si>
-  <si>
     <t>Mac Bones</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>Jack</t>
   </si>
   <si>
-    <t>Moredecaï</t>
-  </si>
-  <si>
     <t>Roberto</t>
   </si>
   <si>
@@ -248,9 +242,6 @@
     <t>Soumral</t>
   </si>
   <si>
-    <t>Yalandhadra</t>
-  </si>
-  <si>
     <t>Jathel</t>
   </si>
   <si>
@@ -258,6 +249,15 @@
   </si>
   <si>
     <t>name_</t>
+  </si>
+  <si>
+    <t>Rolph</t>
+  </si>
+  <si>
+    <t>Mordecaï</t>
+  </si>
+  <si>
+    <t>Yalandhra</t>
   </si>
 </sst>
 </file>
@@ -591,13 +591,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -637,67 +639,67 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +717,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -735,52 +737,52 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -798,7 +800,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -818,37 +820,37 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -866,7 +868,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -886,32 +888,32 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -929,7 +931,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -949,32 +951,32 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -986,13 +988,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1012,32 +1016,32 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1049,15 +1053,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1077,12 +1081,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>